<commit_message>
Final Reports: Group and Individual
</commit_message>
<xml_diff>
--- a/documentation/Timesheets/Timesheet - Combined.xlsx
+++ b/documentation/Timesheets/Timesheet - Combined.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MyAdminSorted\Repository\ELEN7046_Group2_2016\documentation\Timesheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="993"/>
   </bookViews>
@@ -106,7 +101,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="[$-1C09]dd\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -162,17 +157,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,7 +298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,7 +333,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -513,7 +510,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -524,34 +521,33 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="1024" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -560,26 +556,26 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="6">
         <v>42480</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="6">
         <v>42512</v>
       </c>
       <c r="D5" s="2">
@@ -591,10 +587,10 @@
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="6">
         <v>42484</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="6">
         <v>42491</v>
       </c>
       <c r="D6" s="2">
@@ -604,26 +600,26 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="6">
         <v>42491</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="6">
         <v>42498</v>
       </c>
       <c r="D9" s="2">
@@ -635,10 +631,10 @@
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="6">
         <v>42484</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="6">
         <v>42512</v>
       </c>
       <c r="D10" s="2">
@@ -650,10 +646,10 @@
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="6">
         <v>42491</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="6">
         <v>42512</v>
       </c>
       <c r="D11" s="2">
@@ -665,10 +661,10 @@
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="6">
         <v>42512</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="6">
         <v>42512</v>
       </c>
       <c r="D12" s="2">
@@ -678,26 +674,26 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="6">
         <v>42505</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="6">
         <v>42512</v>
       </c>
       <c r="D15" s="2">
@@ -709,10 +705,10 @@
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="6">
         <v>42505</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="6">
         <v>42512</v>
       </c>
       <c r="D16" s="2">
@@ -722,26 +718,26 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="6">
         <v>42512</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="6">
         <v>42540</v>
       </c>
       <c r="D19" s="2">
@@ -751,26 +747,26 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="6">
         <v>42512</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="6">
         <v>42540</v>
       </c>
       <c r="D22" s="2">
@@ -780,26 +776,26 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="6">
         <v>42539</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="6">
         <v>42543</v>
       </c>
       <c r="D25" s="2">
@@ -809,26 +805,26 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="6">
         <v>42484</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="6">
         <v>42552</v>
       </c>
       <c r="D28" s="2">
@@ -840,10 +836,10 @@
       <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="6">
         <v>42547</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="6">
         <v>42552</v>
       </c>
       <c r="D29" s="2">
@@ -853,8 +849,8 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DC : Added duration to timesheet
</commit_message>
<xml_diff>
--- a/documentation/Timesheets/Timesheet - Combined.xlsx
+++ b/documentation/Timesheets/Timesheet - Combined.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MyAdminSorted\Repository\ELEN7046_Group2_2016\documentation\Timesheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="993"/>
   </bookViews>
@@ -90,10 +95,11 @@
     <t xml:space="preserve"> - Component/Unit Testing</t>
   </si>
   <si>
-    <t>Duration</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - Business Case</t>
+  </si>
+  <si>
+    <t>Duration
+(Days)</t>
   </si>
 </sst>
 </file>
@@ -101,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-1C09]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-1C09]dd\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -157,19 +163,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -521,61 +535,61 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="1024" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
+      <c r="D2" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>42480</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>42512</v>
       </c>
       <c r="D5" s="2">
@@ -585,12 +599,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="6">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4">
         <v>42484</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>42491</v>
       </c>
       <c r="D6" s="2">
@@ -600,26 +614,26 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>42491</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>42498</v>
       </c>
       <c r="D9" s="2">
@@ -631,10 +645,10 @@
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>42484</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <v>42512</v>
       </c>
       <c r="D10" s="2">
@@ -646,10 +660,10 @@
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>42491</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>42512</v>
       </c>
       <c r="D11" s="2">
@@ -661,10 +675,10 @@
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>42512</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>42512</v>
       </c>
       <c r="D12" s="2">
@@ -674,26 +688,26 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>42505</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <v>42512</v>
       </c>
       <c r="D15" s="2">
@@ -705,10 +719,10 @@
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>42505</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="4">
         <v>42512</v>
       </c>
       <c r="D16" s="2">
@@ -718,26 +732,26 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <v>42512</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="4">
         <v>42540</v>
       </c>
       <c r="D19" s="2">
@@ -747,26 +761,26 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <v>42512</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="4">
         <v>42540</v>
       </c>
       <c r="D22" s="2">
@@ -776,26 +790,26 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="4">
         <v>42539</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="4">
         <v>42543</v>
       </c>
       <c r="D25" s="2">
@@ -805,26 +819,26 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="4">
         <v>42484</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="4">
         <v>42552</v>
       </c>
       <c r="D28" s="2">
@@ -836,10 +850,10 @@
       <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="4">
         <v>42547</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="4">
         <v>42552</v>
       </c>
       <c r="D29" s="2">
@@ -849,8 +863,8 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
       <c r="D30" s="2"/>
     </row>
   </sheetData>

</xml_diff>